<commit_message>
think input replace is working
</commit_message>
<xml_diff>
--- a/hello.xlsx
+++ b/hello.xlsx
@@ -14,21 +14,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>parameters</t>
   </si>
   <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>elab_method</t>
+  </si>
+  <si>
     <t>scores</t>
   </si>
   <si>
+    <t>{'response': 'build a wall', 'prompt': 'brick', 'originality': 1.0}</t>
+  </si>
+  <si>
+    <t>{'response': 'paper weight', 'prompt': 'brick', 'originality': 1.2}</t>
+  </si>
+  <si>
+    <t>{'response': 'weapon', 'prompt': 'brick', 'originality': 1.4}</t>
+  </si>
+  <si>
     <t>summative</t>
   </si>
   <si>
+    <t>n_examples</t>
+  </si>
+  <si>
+    <t>originality</t>
+  </si>
+  <si>
     <t>version</t>
   </si>
   <si>
+    <t>1.3</t>
+  </si>
+  <si>
     <t>cite</t>
+  </si>
+  <si>
+    <t>Organisciak, P., &amp; Dumas, D. (2020). Open Creativity Scoring. University of Denver. https://openscoring.du.edu</t>
+  </si>
+  <si>
+    <t>Organisciak, P., Acar, S., Dumas, D., &amp; Berthiaume, K. (2023). Beyond semantic distance: Automated scoring of divergent thinking greatly improves with large language models. Thinking Skills and Creativity, 49, 101356. https://doi.org/10.1016/j.tsc.2023.101356</t>
   </si>
 </sst>
 </file>
@@ -360,27 +390,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="E4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>